<commit_message>
job #8257 - Committing files from Ian in "Delivery to OneFact 2017-02-16"
</commit_message>
<xml_diff>
--- a/arc/Issues.xlsx
+++ b/arc/Issues.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="132" windowWidth="22980" windowHeight="9204"/>
+    <workbookView xWindow="0" yWindow="192" windowWidth="22980" windowHeight="9144"/>
   </bookViews>
   <sheets>
     <sheet name="Current Defects in Translator" sheetId="2" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>Issue</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Select where conditions have "SELECTED." and "=="</t>
   </si>
   <si>
-    <t xml:space="preserve">This requires either full interpretation of the OAL condition (a big job) or string editing </t>
-  </si>
-  <si>
     <t>Enumeration literals not rendered correctly</t>
   </si>
   <si>
@@ -64,13 +61,49 @@
     <t>Remnants of C/C++ declarations</t>
   </si>
   <si>
-    <t>Not a problem as a "PARSE ERROR" has been inserted and use will have to manually sort this out anyway</t>
-  </si>
-  <si>
     <t>Event generation parameters are not generated in the correct order</t>
   </si>
   <si>
     <t>Operation call parameters are not generated in the correct order</t>
+  </si>
+  <si>
+    <t>Not required in MASL</t>
+  </si>
+  <si>
+    <t>State action and service/function bodies reference "PARAM."</t>
+  </si>
+  <si>
+    <t>Function calls as part of an expression not translated</t>
+  </si>
+  <si>
+    <t>There appears to be no "continue" in MASL.  Implementing this by elaborated MASL would be very complex</t>
+  </si>
+  <si>
+    <t>Not a problem as a parse error and comment has been inserted and use will have to manually sort this out anyway</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Acceptable</t>
+  </si>
+  <si>
+    <t>Have got rid of SLECTED but "==" and some extraneous "." occurrences remain</t>
+  </si>
+  <si>
+    <t>This allows architecture dependent calls.  Not relevant to MASL.</t>
+  </si>
+  <si>
+    <t>"Control" statement not implemented (Parse error and comment is generated)</t>
+  </si>
+  <si>
+    <t>"Continue" statement not implemented (Parse error and comment is generated)</t>
+  </si>
+  <si>
+    <t>Relationship navigation not yet tested for associative classes and super/sub hierarchies</t>
   </si>
 </sst>
 </file>
@@ -419,19 +452,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C10"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="47.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="95.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="87.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -439,15 +479,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -455,23 +498,26 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -479,40 +525,86 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
         <v>14</v>
       </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>